<commit_message>
added assertion data through excel for test case 7
</commit_message>
<xml_diff>
--- a/Project/testdata/Excel.xlsx
+++ b/Project/testdata/Excel.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,46 +406,73 @@
       <c r="A1" t="str">
         <v>demoname</v>
       </c>
+      <c r="C1" t="str">
+        <v>https://careers.homedepot.com/</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>test</v>
       </c>
+      <c r="C2" t="str">
+        <v>https://corporate.homedepot.com/</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>demotest123@gmail.com</v>
       </c>
+      <c r="C3" t="str">
+        <v>https://corporate.homedepot.com/newsroom</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>998-877-6653</v>
       </c>
+      <c r="C4" t="str">
+        <v>https://corporate.homedepot.com/foundation</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
         <v>Pennsylvania Avenue NW</v>
       </c>
+      <c r="C5" t="str">
+        <v>https://ir.homedepot.com/</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Washington</v>
       </c>
+      <c r="C6" t="str">
+        <v>/c/Government_Customers</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>DC</v>
       </c>
+      <c r="C7" t="str">
+        <v>/c/suppliers_and_providers</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>20004</v>
       </c>
+      <c r="C8" t="str">
+        <v>https://www.homedepot.com/c/SF_MS_The_Home_Depot_Affiliate_Program</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
         <v>Rent</v>
       </c>
+      <c r="C9" t="str">
+        <v>https://ecoactions.homedepot.com/</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -459,7 +486,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added comments for testcase 7 and 8
</commit_message>
<xml_diff>
--- a/Project/testdata/Excel.xlsx
+++ b/Project/testdata/Excel.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +409,9 @@
       <c r="C1" t="str">
         <v>https://careers.homedepot.com/</v>
       </c>
+      <c r="D1" t="str">
+        <v>CREDIT CARD SERVICES</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -486,7 +489,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added assert in testcase 8
</commit_message>
<xml_diff>
--- a/Project/testdata/Excel.xlsx
+++ b/Project/testdata/Excel.xlsx
@@ -420,6 +420,9 @@
       <c r="C2" t="str">
         <v>https://corporate.homedepot.com/</v>
       </c>
+      <c r="D2" t="str">
+        <v>Home Depot Credit Card Application</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -427,6 +430,9 @@
       </c>
       <c r="C3" t="str">
         <v>https://corporate.homedepot.com/newsroom</v>
+      </c>
+      <c r="D3" t="str">
+        <v>https://citiretailservices.citibankonline.com/apply/home-depot-credit-card?app=UNSOL&amp;siteId=PLCN_HOMEDEPOT&amp;sc=30005&amp;cmp=A~E~D~R~A~9~ZZZ0~AI~HD~ZZ_D3T</v>
       </c>
     </row>
     <row r="4">

</xml_diff>